<commit_message>
Reporte Normativa - instancia general implementado y funcional
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-reportes-normativa.xlsx
+++ b/assets/info/plantilla-reportes-normativa.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Plenarias" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Normativa" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -33,34 +33,34 @@
     <t xml:space="preserve">FECHA REGISTRO</t>
   </si>
   <si>
-    <t xml:space="preserve">FECHA PLENARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTANCIA DE SEGUIMIENTO</t>
+    <t xml:space="preserve">FECHA NORMATIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTANCIA</t>
   </si>
   <si>
     <t xml:space="preserve">DEPARTAMENTO</t>
   </si>
   <si>
-    <t xml:space="preserve">MUNICIPIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUNTOS DE LA AGENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUMPLIMIENTO DE LA AGENDA [%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCRIPCION DEL ASUNTO QUE SE DEJO SIN TRATAMIENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUNTOS VARIOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERO Y NOMBRE DE LA NORMA QUE INGRESO SIN ESTAR EN AGENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO DE PLENARIA</t>
+    <t xml:space="preserve">MUNICIPIO – DEPARTAMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJETO DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMA 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMA 2</t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
@@ -362,13 +362,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>985680</xdr:colOff>
+      <xdr:colOff>983880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -381,8 +381,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="314640"/>
-          <a:ext cx="3589200" cy="1122120"/>
+          <a:off x="66600" y="315000"/>
+          <a:ext cx="3587400" cy="1120320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -408,9 +408,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>919080</xdr:colOff>
+      <xdr:colOff>917280</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -424,7 +424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3522600" cy="1255680"/>
+          <a:ext cx="3520800" cy="1253880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -450,9 +450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>726480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>226800</xdr:rowOff>
+      <xdr:rowOff>225000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -466,7 +466,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3331800" cy="1303200"/>
+          <a:ext cx="3330000" cy="1301400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -486,30 +486,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="43.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="44.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="37.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="34.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="43.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="4" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="59.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="43.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="44.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="37.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="34.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="41.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="37.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="4" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -525,21 +525,29 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
@@ -563,10 +571,10 @@
       <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="10" t="s">
@@ -585,29 +593,31 @@
         <v>14</v>
       </c>
       <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6:G1048576">
+  <conditionalFormatting sqref="I6:I1048576">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",I6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G1048576 G1:G4 H5">
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I1048576 I1:I4 J5">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="1">
-      <formula>NOT(ISERROR(SEARCH("Censo",G1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G1048576 G1:G4 H5">
+      <formula>NOT(ISERROR(SEARCH("Censo",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I1048576 I1:I4 J5">
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>